<commit_message>
cross validation regresion logistica
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,245 +436,91 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Exactitud</t>
+          <t>precision_macro</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Precisión</t>
+          <t>recall_macro</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Matriz de confusión</t>
+          <t>precision_micro</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>fpr_micro</t>
+          <t>recall_micro</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>tpr_micro</t>
+          <t>f1_macro</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>roc_auc_micro</t>
+          <t>accuracy</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>fpr</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>tpr</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>roc_auc</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Regresión Logística RGB</t>
+        </is>
       </c>
       <c r="B2" t="n">
-        <v>38</v>
+        <v>0.37615196453386</v>
       </c>
       <c r="C2" t="n">
-        <v>46.11111111111111</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>[[5 3 0 2 0]
- [2 4 0 1 3]
- [0 4 3 0 3]
- [1 3 1 3 2]
- [2 4 0 0 4]]</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>[0.    0.02  0.12  0.345 1.   ]</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>[0.   0.1  0.28 0.68 1.  ]</t>
-        </is>
+        <v>0.3703476412684976</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.3788135593220339</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.3788135593220339</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.3689149283290373</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6782</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>{0: array([0.   , 0.025, 0.075, 0.225, 1.   ]), 1: array([0.   , 0.   , 0.225, 0.6  , 1.   ]), 2: array([0.   , 0.025, 0.225, 1.   ]), 3: array([0.   , 0.025, 0.075, 0.25 , 1.   ]), 4: array([0.   , 0.05 , 0.2  , 0.425, 1.   ])}</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>{0: array([0. , 0. , 0.2, 0.6, 1. ]), 1: array([0. , 0.1, 0.2, 0.8, 1. ]), 2: array([0. , 0.3, 0.5, 1. ]), 3: array([0. , 0.2, 0.3, 0.8, 1. ]), 4: array([0. , 0.2, 0.4, 0.7, 1. ])}</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>{0: np.float64(0.6850000000000002), 1: np.float64(0.58125), 2: np.float64(0.665), 3: np.float64(0.78625), 4: np.float64(0.6625)}</t>
-        </is>
-      </c>
+        <v>0.3788135593220339</v>
+      </c>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Regresión Logística RGB</t>
+        </is>
       </c>
       <c r="B3" t="n">
-        <v>38</v>
+        <v>0.37615196453386</v>
       </c>
       <c r="C3" t="n">
-        <v>46.11111111111111</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>[[5 3 0 2 0]
- [2 4 0 1 3]
- [0 4 3 0 3]
- [1 3 1 3 2]
- [2 4 0 0 4]]</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>[0.    0.02  0.12  0.345 1.   ]</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>[0.   0.1  0.28 0.68 1.  ]</t>
-        </is>
+        <v>0.3703476412684976</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.3788135593220339</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.3788135593220339</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.3689149283290373</v>
       </c>
       <c r="G3" t="n">
-        <v>0.6782</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>{0: array([0.   , 0.025, 0.075, 0.225, 1.   ]), 1: array([0.   , 0.   , 0.225, 0.6  , 1.   ]), 2: array([0.   , 0.025, 0.225, 1.   ]), 3: array([0.   , 0.025, 0.075, 0.25 , 1.   ]), 4: array([0.   , 0.05 , 0.2  , 0.425, 1.   ])}</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>{0: array([0. , 0. , 0.2, 0.6, 1. ]), 1: array([0. , 0.1, 0.2, 0.8, 1. ]), 2: array([0. , 0.3, 0.5, 1. ]), 3: array([0. , 0.2, 0.3, 0.8, 1. ]), 4: array([0. , 0.2, 0.4, 0.7, 1. ])}</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>{0: np.float64(0.6850000000000002), 1: np.float64(0.58125), 2: np.float64(0.665), 3: np.float64(0.78625), 4: np.float64(0.6625)}</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>prueba</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>38</v>
-      </c>
-      <c r="C4" t="n">
-        <v>46.11111111111111</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>[[5 3 0 2 0]
- [2 4 0 1 3]
- [0 4 3 0 3]
- [1 3 1 3 2]
- [2 4 0 0 4]]</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>[0.    0.02  0.12  0.345 1.   ]</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>[0.   0.1  0.28 0.68 1.  ]</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>0.6782</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>{0: array([0.   , 0.025, 0.075, 0.225, 1.   ]), 1: array([0.   , 0.   , 0.225, 0.6  , 1.   ]), 2: array([0.   , 0.025, 0.225, 1.   ]), 3: array([0.   , 0.025, 0.075, 0.25 , 1.   ]), 4: array([0.   , 0.05 , 0.2  , 0.425, 1.   ])}</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>{0: array([0. , 0. , 0.2, 0.6, 1. ]), 1: array([0. , 0.1, 0.2, 0.8, 1. ]), 2: array([0. , 0.3, 0.5, 1. ]), 3: array([0. , 0.2, 0.3, 0.8, 1. ]), 4: array([0. , 0.2, 0.4, 0.7, 1. ])}</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>{0: np.float64(0.6850000000000002), 1: np.float64(0.58125), 2: np.float64(0.665), 3: np.float64(0.78625), 4: np.float64(0.6625)}</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>KNN</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>38</v>
-      </c>
-      <c r="C5" t="n">
-        <v>46.11111111111111</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>[[5 3 0 2 0]
- [2 4 0 1 3]
- [0 4 3 0 3]
- [1 3 1 3 2]
- [2 4 0 0 4]]</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>[0.    0.02  0.12  0.345 1.   ]</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>[0.   0.1  0.28 0.68 1.  ]</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>0.6782</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>{0: array([0.   , 0.025, 0.075, 0.225, 1.   ]), 1: array([0.   , 0.   , 0.225, 0.6  , 1.   ]), 2: array([0.   , 0.025, 0.225, 1.   ]), 3: array([0.   , 0.025, 0.075, 0.25 , 1.   ]), 4: array([0.   , 0.05 , 0.2  , 0.425, 1.   ])}</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>{0: array([0. , 0. , 0.2, 0.6, 1. ]), 1: array([0. , 0.1, 0.2, 0.8, 1. ]), 2: array([0. , 0.3, 0.5, 1. ]), 3: array([0. , 0.2, 0.3, 0.8, 1. ]), 4: array([0. , 0.2, 0.4, 0.7, 1. ])}</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>{0: np.float64(0.6850000000000002), 1: np.float64(0.58125), 2: np.float64(0.665), 3: np.float64(0.78625), 4: np.float64(0.6625)}</t>
-        </is>
-      </c>
+        <v>0.3788135593220339</v>
+      </c>
+      <c r="H3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>